<commit_message>
Pruefung des Quellenverzeichnisses, obb nicht verwendete Quellen vorlagen. Alle angegebenen Quellen werden verwendet. Chatprotokoll mit ChatGPT eingefügt
</commit_message>
<xml_diff>
--- a/src/main/3 insert Entgeltdaten/2 Tarif.xlsx
+++ b/src/main/3 insert Entgeltdaten/2 Tarif.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\test\testdaten_insert_tarif\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\3 insert Entgeltdaten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D500B873-F3EF-4069-BE14-B666F61F8904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12F9B58-ABB7-4BA7-8E65-2C718D25688B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="2160" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -382,7 +382,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>